<commit_message>
commit 9 June 2016
</commit_message>
<xml_diff>
--- a/data/PHINDA_MATERNITY_DATA.xlsx
+++ b/data/PHINDA_MATERNITY_DATA.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbalm_000\Documents\Files\Leopards\Munyawana Leopard Project\Phinda\Phinda demog files_FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RossTyzackPitman/Documents/OneDrive/PhD/Data/R_Database/R_PROJECTS/PhD_Chapter3/MSE_Paper/LEOPARD-MP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +38,7 @@
     <author>gbalme@panthera.org</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Female</t>
   </si>
@@ -136,6 +142,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
 </sst>
 </file>
@@ -295,9 +304,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -330,9 +339,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -514,30 +523,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.83203125" style="5"/>
     <col min="9" max="9" width="21" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="6" customWidth="1"/>
+    <col min="10" max="11" width="8.5" style="5" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="6" customWidth="1"/>
     <col min="13" max="13" width="16" style="5" customWidth="1"/>
     <col min="14" max="14" width="16" style="6" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="6"/>
-    <col min="16" max="16384" width="9.140625" style="5"/>
+    <col min="15" max="15" width="8.83203125" style="6"/>
+    <col min="16" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -574,7 +582,7 @@
       </c>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -620,7 +628,7 @@
       </c>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -666,7 +674,7 @@
       </c>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -708,7 +716,7 @@
       </c>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -751,7 +759,7 @@
       </c>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -794,7 +802,7 @@
       </c>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -823,12 +831,23 @@
         <v>3.043835616438356</v>
       </c>
       <c r="J7" s="12"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="8">
+        <f>L3/SQRT(L6)</f>
+        <v>0.12781493682992215</v>
+      </c>
+      <c r="M7" s="8">
+        <f t="shared" ref="M7:N7" si="2">M3/SQRT(M6)</f>
+        <v>0.19615628990927958</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.19957930816923325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -859,7 +878,7 @@
       <c r="J8" s="12"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -889,7 +908,7 @@
       <c r="J9" s="12"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -898,17 +917,17 @@
         <v>30</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:D10" si="2">SUM(C2:C9)</f>
+        <f t="shared" ref="C10:D10" si="3">SUM(C2:C9)</f>
         <v>52</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34.659999999999997</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>

</xml_diff>